<commit_message>
add: Prepareness for experiments
Former-commit-id: e6a7773c7edcfe845f93fda171bb50a4dea1c1e1
Former-commit-id: 5ef2f3aeb216ae607a608f5dfd306fa969734f9d
</commit_message>
<xml_diff>
--- a/note/SIPLIB_experiments.xlsx
+++ b/note/SIPLIB_experiments.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t xml:space="preserve">SIPLIBv1 </t>
   </si>
@@ -59,14 +59,162 @@
   </si>
   <si>
     <t xml:space="preserve">DCAP_2_3_3_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500/1000/10000/100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21600 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCAP_2_4_3_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCAP_3_3_2_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCAP_3_4_2_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D0_50_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D1_50_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D2_50_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D3_50_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D1_100_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D0_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100/1000/10000/100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=10000 can’t be generated in labtop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D1_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D2_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D3_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D0_100_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D1_100_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D2_100_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPs_D3_100_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZES_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZES_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZES_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZES_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/100/1000/10000/100000/1000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=1000000 can’t be generated in labtop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMKP_120_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMKP_120_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/100/1000/10000/100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=100000 can’t be generated in labtop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIP/TIME_LIM should be set lower than the default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSLP_5_25_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSLP_5_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSLP_10_50_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50/100/500/1000/2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSLP_15_45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSLP_15_45_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_FallWD_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/100/1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_FallWE_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_SpringWD_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_SpringWE_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_SummerWD_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_SummerWE_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_WinterWD_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCW_WinterWE_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -140,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,8 +305,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -178,17 +338,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,36 +398,62 @@
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>1000</v>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="n">
-        <v>10000</v>
-      </c>
+      <c r="A18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="n">
-        <v>100000</v>
-      </c>
+      <c r="A19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -309,17 +496,174 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="C17:C24"/>
+    <mergeCell ref="D17:D24"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -335,17 +679,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C17:C20"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -361,17 +782,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C20"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -387,17 +914,136 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>42134</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -413,17 +1059,145 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6"/>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>